<commit_message>
[PHOENIX-6079] completed entering contact in info for complaint registration
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contactInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="grievanceDetails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>dataName</t>
   </si>
@@ -43,13 +43,43 @@
   </si>
   <si>
     <t>citizenName</t>
+  </si>
+  <si>
+    <t>grievanceDetails</t>
+  </si>
+  <si>
+    <t>Public Health and Sanitation</t>
+  </si>
+  <si>
+    <t>grievanceCategory</t>
+  </si>
+  <si>
+    <t>grievanceType</t>
+  </si>
+  <si>
+    <t>Mosquito menace</t>
+  </si>
+  <si>
+    <t>Deadly deseases are spreading because of mosquitoes</t>
+  </si>
+  <si>
+    <t>Abbas Nagar-m - Election Ward No. 1</t>
+  </si>
+  <si>
+    <t>grievanceLocation</t>
+  </si>
+  <si>
+    <t>locationLandmark</t>
+  </si>
+  <si>
+    <t>Near Vinayaka Temple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +94,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,9 +124,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -394,13 +434,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -450,13 +491,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[PHOENIX-5910] added search trade feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[PHOENIX-5910] changes in search trade license and approval details
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
@@ -60,9 +60,6 @@
     <t>Mosquito menace</t>
   </si>
   <si>
-    <t>Deadly deseases are spreading because of mosquitoes</t>
-  </si>
-  <si>
     <t>Abbas Nagar-m - Election Ward No. 1</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Near Vinayaka Temple</t>
+  </si>
+  <si>
+    <t>Deadly diseases are spreading because of mosquitoes</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +521,10 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -538,13 +538,13 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-6061] Code Refactoring of Grievances and council management
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/grievancesTestData.xlsx
@@ -54,9 +54,6 @@
     <t>grievanceType</t>
   </si>
   <si>
-    <t>Abbas Nagar-m - Election Ward No. 1</t>
-  </si>
-  <si>
     <t>grievanceLocation</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>No street light past 3 days</t>
+  </si>
+  <si>
+    <t>Aavanthi Nagar</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
@@ -528,13 +528,13 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -542,22 +542,22 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>